<commit_message>
Implemented conversion of binary tree into array and vice-versa
</commit_message>
<xml_diff>
--- a/doc/Quora 500.xlsx
+++ b/doc/Quora 500.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4835" uniqueCount="523">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4834" uniqueCount="523">
   <si>
     <t>Array</t>
   </si>
@@ -2107,803 +2107,877 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:L21"/>
+  <dimension ref="A1:M21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="5" style="28" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32" style="28" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.28515625" style="31" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13" style="31" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="9.140625" style="28"/>
-    <col min="7" max="7" width="14.85546875" style="28" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.5703125" style="24" customWidth="1"/>
-    <col min="9" max="9" width="15" style="25" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16" style="26" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.85546875" style="28" customWidth="1"/>
-    <col min="12" max="12" width="12.42578125" style="28" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="28"/>
+    <col min="1" max="1" width="6.42578125" style="28" customWidth="1"/>
+    <col min="2" max="2" width="5" style="28" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32" style="28" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15" style="25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.85546875" style="31" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11" style="31" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.7109375" style="28" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" style="28"/>
+    <col min="9" max="9" width="12" style="28" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.5703125" style="24" customWidth="1"/>
+    <col min="11" max="11" width="16" style="26" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.85546875" style="28" customWidth="1"/>
+    <col min="13" max="13" width="12.42578125" style="28" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="28"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="15" customFormat="1" ht="15.75">
-      <c r="A1" s="20"/>
-      <c r="B1" s="20" t="s">
+    <row r="1" spans="1:13" s="15" customFormat="1" ht="15.75">
+      <c r="B1" s="20"/>
+      <c r="C1" s="20" t="s">
         <v>377</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="D1" s="21" t="s">
+        <v>521</v>
+      </c>
+      <c r="E1" s="16" t="s">
         <v>518</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="F1" s="16" t="s">
         <v>517</v>
       </c>
-      <c r="E1" s="16" t="s">
+      <c r="G1" s="16" t="s">
         <v>374</v>
       </c>
-      <c r="F1" s="16" t="s">
+      <c r="H1" s="16" t="s">
         <v>375</v>
       </c>
-      <c r="G1" s="16" t="s">
+      <c r="I1" s="16" t="s">
         <v>376</v>
       </c>
-      <c r="H1" s="19" t="s">
+      <c r="J1" s="19" t="s">
         <v>520</v>
       </c>
-      <c r="I1" s="21" t="s">
-        <v>521</v>
-      </c>
-      <c r="J1" s="19" t="s">
+      <c r="K1" s="19" t="s">
         <v>519</v>
       </c>
-      <c r="K1" s="19" t="s">
+      <c r="L1" s="19" t="s">
         <v>396</v>
       </c>
-      <c r="L1" s="19" t="s">
+      <c r="M1" s="19" t="s">
         <v>397</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="15">
-      <c r="A2" s="22" t="s">
+    <row r="2" spans="1:13" ht="15">
+      <c r="A2" s="28">
+        <v>1</v>
+      </c>
+      <c r="B2" s="22" t="s">
         <v>367</v>
       </c>
-      <c r="B2" s="23" t="s">
+      <c r="C2" s="23" t="s">
         <v>167</v>
       </c>
-      <c r="C2" s="22">
-        <f>COUNTIF(All_unique!B:B,B2)</f>
+      <c r="D2" s="25">
+        <v>4</v>
+      </c>
+      <c r="E2" s="22">
+        <f>COUNTIF(All_unique!B:B,C2)</f>
         <v>12</v>
       </c>
-      <c r="D2" s="22">
-        <f>COUNTIF(All!B:B,B2)</f>
+      <c r="F2" s="22">
+        <f>COUNTIF(All!B:B,C2)</f>
         <v>14</v>
       </c>
-      <c r="E2" s="22">
+      <c r="G2" s="22">
         <f>Details_old!F293</f>
         <v>11</v>
       </c>
-      <c r="F2" s="22">
+      <c r="H2" s="22">
         <f>Details_old!G293</f>
         <v>0</v>
       </c>
-      <c r="G2" s="22">
+      <c r="I2" s="22">
         <f>Details_old!H293</f>
         <v>11</v>
       </c>
-      <c r="H2" s="24">
-        <f>E2*10/60</f>
+      <c r="J2" s="24">
+        <f t="shared" ref="J2:J19" si="0">G2*10/60</f>
         <v>1.8333333333333333</v>
       </c>
-      <c r="I2" s="25" t="s">
-        <v>522</v>
-      </c>
-      <c r="J2" s="26" t="s">
+      <c r="K2" s="26" t="s">
         <v>354</v>
       </c>
-      <c r="K2" s="27">
+      <c r="L2" s="27">
         <v>0.41666666666666669</v>
       </c>
-      <c r="L2" s="27">
+      <c r="M2" s="27">
         <v>0.5</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="15">
-      <c r="A3" s="22" t="s">
+    <row r="3" spans="1:13" ht="15">
+      <c r="A3" s="28">
+        <v>2</v>
+      </c>
+      <c r="B3" s="22" t="s">
         <v>366</v>
       </c>
-      <c r="B3" s="23" t="s">
+      <c r="C3" s="23" t="s">
         <v>126</v>
       </c>
-      <c r="C3" s="22">
-        <f>COUNTIF(All_unique!B:B,B3)</f>
+      <c r="E3" s="22">
+        <f>COUNTIF(All_unique!B:B,C3)</f>
         <v>48</v>
       </c>
-      <c r="D3" s="22">
-        <f>COUNTIF(All!B:B,B3)</f>
+      <c r="F3" s="22">
+        <f>COUNTIF(All!B:B,C3)</f>
         <v>49</v>
       </c>
-      <c r="E3" s="22">
+      <c r="G3" s="22">
         <f>Details_old!F251</f>
         <v>41</v>
       </c>
-      <c r="F3" s="22">
+      <c r="H3" s="22">
         <f>Details_old!G251</f>
         <v>0</v>
       </c>
-      <c r="G3" s="22">
+      <c r="I3" s="22">
         <f>Details_old!H251</f>
         <v>41</v>
       </c>
-      <c r="H3" s="24">
-        <f>E3*10/60</f>
+      <c r="J3" s="24">
+        <f t="shared" si="0"/>
         <v>6.833333333333333</v>
       </c>
-      <c r="J3" s="26" t="s">
+      <c r="K3" s="26" t="s">
         <v>354</v>
       </c>
-      <c r="K3" s="27">
+      <c r="L3" s="27">
         <v>0.5</v>
       </c>
-      <c r="L3" s="27">
+      <c r="M3" s="27">
         <v>0.625</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="15">
-      <c r="A4" s="22" t="s">
+    <row r="4" spans="1:13" ht="15">
+      <c r="A4" s="28">
+        <v>3</v>
+      </c>
+      <c r="B4" s="22" t="s">
         <v>355</v>
       </c>
-      <c r="B4" s="29" t="s">
+      <c r="C4" s="29" t="s">
         <v>180</v>
       </c>
-      <c r="C4" s="22">
-        <f>COUNTIF(All_unique!B:B,B4)</f>
+      <c r="E4" s="22">
+        <f>COUNTIF(All_unique!B:B,C4)</f>
         <v>41</v>
       </c>
-      <c r="D4" s="22">
-        <f>COUNTIF(All!B:B,B4)</f>
+      <c r="F4" s="22">
+        <f>COUNTIF(All!B:B,C4)</f>
         <v>56</v>
       </c>
-      <c r="E4" s="22">
+      <c r="G4" s="22">
         <f>Details_old!F2</f>
         <v>45</v>
       </c>
-      <c r="F4" s="22">
+      <c r="H4" s="22">
         <f>Details_old!G2</f>
         <v>42</v>
       </c>
-      <c r="G4" s="22">
+      <c r="I4" s="22">
         <f>Details_old!H2</f>
         <v>3</v>
       </c>
-      <c r="H4" s="24">
-        <f>E4*10/60</f>
+      <c r="J4" s="24">
+        <f t="shared" si="0"/>
         <v>7.5</v>
       </c>
-      <c r="J4" s="26" t="s">
+      <c r="K4" s="26" t="s">
         <v>354</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="15">
-      <c r="A5" s="22" t="s">
+    <row r="5" spans="1:13" ht="15">
+      <c r="A5" s="28">
+        <v>4</v>
+      </c>
+      <c r="B5" s="22" t="s">
         <v>356</v>
       </c>
-      <c r="B5" s="29" t="s">
+      <c r="C5" s="29" t="s">
         <v>337</v>
       </c>
-      <c r="C5" s="22">
-        <f>COUNTIF(All_unique!B:B,B5)</f>
+      <c r="D5" s="25">
         <v>1</v>
       </c>
-      <c r="D5" s="22">
-        <f>COUNTIF(All!B:B,B5)</f>
+      <c r="E5" s="22">
+        <f>COUNTIF(All_unique!B:B,C5)</f>
+        <v>1</v>
+      </c>
+      <c r="F5" s="22">
+        <f>COUNTIF(All!B:B,C5)</f>
         <v>7</v>
       </c>
-      <c r="E5" s="22">
+      <c r="G5" s="22">
         <f>Details_old!F48</f>
         <v>5</v>
       </c>
-      <c r="F5" s="22">
+      <c r="H5" s="22">
         <f>Details_old!G48</f>
         <v>4</v>
       </c>
-      <c r="G5" s="22">
+      <c r="I5" s="22">
         <f>Details_old!H48</f>
         <v>1</v>
       </c>
-      <c r="H5" s="24">
-        <f>E5*10/60</f>
+      <c r="J5" s="24">
+        <f t="shared" si="0"/>
         <v>0.83333333333333337</v>
       </c>
-      <c r="J5" s="26" t="s">
+      <c r="K5" s="26" t="s">
         <v>354</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="15">
-      <c r="A6" s="22" t="s">
+    <row r="6" spans="1:13" ht="15">
+      <c r="A6" s="28">
+        <v>5</v>
+      </c>
+      <c r="B6" s="22" t="s">
         <v>362</v>
       </c>
-      <c r="B6" s="23" t="s">
+      <c r="C6" s="23" t="s">
         <v>332</v>
       </c>
-      <c r="C6" s="22">
-        <f>COUNTIF(All_unique!B:B,B6)</f>
+      <c r="D6" s="25">
+        <v>2</v>
+      </c>
+      <c r="E6" s="22">
+        <f>COUNTIF(All_unique!B:B,C6)</f>
         <v>5</v>
       </c>
-      <c r="D6" s="22">
-        <f>COUNTIF(All!B:B,B6)</f>
+      <c r="F6" s="22">
+        <f>COUNTIF(All!B:B,C6)</f>
         <v>9</v>
       </c>
-      <c r="E6" s="22">
+      <c r="G6" s="22">
         <f>Details_old!F172</f>
         <v>7</v>
       </c>
-      <c r="F6" s="22">
+      <c r="H6" s="22">
         <f>Details_old!G172</f>
         <v>7</v>
       </c>
-      <c r="G6" s="22">
+      <c r="I6" s="22">
         <f>Details_old!H172</f>
         <v>0</v>
       </c>
-      <c r="H6" s="24">
-        <f t="shared" ref="H6:H19" si="0">E6*10/60</f>
+      <c r="J6" s="24">
+        <f t="shared" si="0"/>
         <v>1.1666666666666667</v>
       </c>
-      <c r="J6" s="26" t="s">
+      <c r="K6" s="26" t="s">
         <v>354</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="15">
-      <c r="A7" s="22" t="s">
+    <row r="7" spans="1:13" ht="15">
+      <c r="A7" s="28">
+        <v>6</v>
+      </c>
+      <c r="B7" s="22" t="s">
         <v>357</v>
       </c>
-      <c r="B7" s="29" t="s">
+      <c r="C7" s="29" t="s">
         <v>93</v>
       </c>
-      <c r="C7" s="22">
-        <f>COUNTIF(All_unique!B:B,B7)</f>
+      <c r="D7" s="25">
+        <v>3</v>
+      </c>
+      <c r="E7" s="22">
+        <f>COUNTIF(All_unique!B:B,C7)</f>
         <v>11</v>
       </c>
-      <c r="D7" s="22">
-        <f>COUNTIF(All!B:B,B7)</f>
+      <c r="F7" s="22">
+        <f>COUNTIF(All!B:B,C7)</f>
         <v>13</v>
       </c>
-      <c r="E7" s="22">
+      <c r="G7" s="22">
         <f>Details_old!F54</f>
         <v>12</v>
       </c>
-      <c r="F7" s="22">
+      <c r="H7" s="22">
         <f>Details_old!G54</f>
         <v>0</v>
       </c>
-      <c r="G7" s="22">
+      <c r="I7" s="22">
         <f>Details_old!H54</f>
         <v>12</v>
       </c>
-      <c r="H7" s="24">
-        <f>E7*10/60</f>
+      <c r="J7" s="24">
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="J7" s="26" t="s">
+      <c r="K7" s="26" t="s">
         <v>354</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="15">
-      <c r="A8" s="22" t="s">
+    <row r="8" spans="1:13" ht="15">
+      <c r="A8" s="28">
+        <v>7</v>
+      </c>
+      <c r="B8" s="22" t="s">
         <v>358</v>
       </c>
-      <c r="B8" s="30" t="s">
+      <c r="C8" s="30" t="s">
         <v>178</v>
       </c>
-      <c r="C8" s="22">
-        <f>COUNTIF(All_unique!B:B,B8)</f>
+      <c r="D8" s="25">
+        <v>7</v>
+      </c>
+      <c r="E8" s="22">
+        <f>COUNTIF(All_unique!B:B,C8)</f>
         <v>2</v>
       </c>
-      <c r="D8" s="22">
-        <f>COUNTIF(All!B:B,B8)</f>
+      <c r="F8" s="22">
+        <f>COUNTIF(All!B:B,C8)</f>
         <v>30</v>
       </c>
-      <c r="E8" s="22">
+      <c r="G8" s="22">
         <f>Details_old!F67</f>
         <v>22</v>
       </c>
-      <c r="F8" s="22">
+      <c r="H8" s="22">
         <f>Details_old!G67</f>
         <v>0</v>
       </c>
-      <c r="G8" s="22">
+      <c r="I8" s="22">
         <f>Details_old!H67</f>
         <v>22</v>
       </c>
-      <c r="H8" s="24">
-        <f>E8*10/60</f>
+      <c r="J8" s="24">
+        <f t="shared" si="0"/>
         <v>3.6666666666666665</v>
       </c>
-      <c r="J8" s="26" t="s">
+      <c r="K8" s="26" t="s">
         <v>354</v>
       </c>
-      <c r="K8" s="27">
+      <c r="L8" s="27">
         <v>0.625</v>
       </c>
-      <c r="L8" s="27">
+      <c r="M8" s="27">
         <v>0.70833333333333337</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="15">
-      <c r="A9" s="22" t="s">
+    <row r="9" spans="1:13" ht="15">
+      <c r="A9" s="28">
+        <v>8</v>
+      </c>
+      <c r="B9" s="22" t="s">
         <v>371</v>
       </c>
-      <c r="B9" s="23" t="s">
+      <c r="C9" s="23" t="s">
         <v>298</v>
       </c>
-      <c r="C9" s="22">
-        <f>COUNTIF(All_unique!B:B,B9)</f>
+      <c r="D9" s="25">
+        <v>6</v>
+      </c>
+      <c r="E9" s="22">
+        <f>COUNTIF(All_unique!B:B,C9)</f>
         <v>5</v>
       </c>
-      <c r="D9" s="22">
-        <f>COUNTIF(All!B:B,B9)</f>
+      <c r="F9" s="22">
+        <f>COUNTIF(All!B:B,C9)</f>
         <v>17</v>
       </c>
-      <c r="E9" s="22">
+      <c r="G9" s="22">
         <f>Details_old!F410</f>
         <v>13</v>
       </c>
-      <c r="F9" s="22">
+      <c r="H9" s="22">
         <f>Details_old!G410</f>
         <v>0</v>
       </c>
-      <c r="G9" s="22">
+      <c r="I9" s="22">
         <f>Details_old!H410</f>
         <v>13</v>
       </c>
-      <c r="H9" s="24">
+      <c r="J9" s="24">
         <f t="shared" si="0"/>
         <v>2.1666666666666665</v>
       </c>
-      <c r="J9" s="26" t="s">
+      <c r="K9" s="26" t="s">
         <v>354</v>
       </c>
-      <c r="K9" s="27">
+      <c r="L9" s="27">
         <v>0.70833333333333337</v>
       </c>
-      <c r="L9" s="27">
+      <c r="M9" s="27">
         <v>0.75</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="15">
-      <c r="A10" s="22" t="s">
+    <row r="10" spans="1:13" ht="15">
+      <c r="A10" s="28">
+        <v>9</v>
+      </c>
+      <c r="B10" s="22" t="s">
         <v>363</v>
       </c>
-      <c r="B10" s="23" t="s">
+      <c r="C10" s="23" t="s">
         <v>239</v>
       </c>
-      <c r="C10" s="22">
-        <f>COUNTIF(All_unique!B:B,B10)</f>
+      <c r="D10" s="25">
+        <v>5</v>
+      </c>
+      <c r="E10" s="22">
+        <f>COUNTIF(All_unique!B:B,C10)</f>
         <v>2</v>
       </c>
-      <c r="D10" s="22">
-        <f>COUNTIF(All!B:B,B10)</f>
+      <c r="F10" s="22">
+        <f>COUNTIF(All!B:B,C10)</f>
         <v>16</v>
       </c>
-      <c r="E10" s="22">
+      <c r="G10" s="22">
         <f>Details_old!F180</f>
         <v>15</v>
       </c>
-      <c r="F10" s="22">
+      <c r="H10" s="22">
         <f>Details_old!G180</f>
         <v>1</v>
       </c>
-      <c r="G10" s="22">
+      <c r="I10" s="22">
         <f>Details_old!H180</f>
         <v>14</v>
       </c>
-      <c r="H10" s="24">
+      <c r="J10" s="24">
         <f t="shared" si="0"/>
         <v>2.5</v>
       </c>
-      <c r="J10" s="26" t="s">
+      <c r="K10" s="26" t="s">
         <v>354</v>
       </c>
-      <c r="K10" s="27">
+      <c r="L10" s="27">
         <v>0.75</v>
       </c>
-      <c r="L10" s="27">
+      <c r="M10" s="27">
         <v>0.83333333333333337</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="15">
-      <c r="A11" s="22" t="s">
+    <row r="11" spans="1:13" ht="15">
+      <c r="A11" s="28">
+        <v>10</v>
+      </c>
+      <c r="B11" s="22" t="s">
         <v>360</v>
       </c>
-      <c r="B11" s="23" t="s">
+      <c r="C11" s="23" t="s">
         <v>339</v>
       </c>
-      <c r="C11" s="22">
-        <f>COUNTIF(All_unique!B:B,B11)</f>
+      <c r="E11" s="22">
+        <f>COUNTIF(All_unique!B:B,C11)</f>
         <v>22</v>
       </c>
-      <c r="D11" s="22">
-        <f>COUNTIF(All!B:B,B11)</f>
+      <c r="F11" s="22">
+        <f>COUNTIF(All!B:B,C11)</f>
         <v>27</v>
       </c>
-      <c r="E11" s="22">
+      <c r="G11" s="22">
         <f>Details_old!F125</f>
         <v>16</v>
       </c>
-      <c r="F11" s="22">
+      <c r="H11" s="22">
         <f>Details_old!G125</f>
         <v>1</v>
       </c>
-      <c r="G11" s="22">
+      <c r="I11" s="22">
         <f>Details_old!H125</f>
         <v>15</v>
       </c>
-      <c r="H11" s="24">
+      <c r="J11" s="24">
         <f t="shared" si="0"/>
         <v>2.6666666666666665</v>
       </c>
-      <c r="J11" s="26" t="s">
+      <c r="K11" s="26" t="s">
         <v>354</v>
       </c>
-      <c r="K11" s="27">
+      <c r="L11" s="27">
         <v>0.83333333333333337</v>
       </c>
-      <c r="L11" s="27">
+      <c r="M11" s="27">
         <v>0.91666666666666663</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="15">
-      <c r="A12" s="22" t="s">
+    <row r="12" spans="1:13" ht="15">
+      <c r="A12" s="28">
+        <v>11</v>
+      </c>
+      <c r="B12" s="22" t="s">
         <v>365</v>
       </c>
-      <c r="B12" s="23" t="s">
+      <c r="C12" s="23" t="s">
         <v>105</v>
       </c>
-      <c r="C12" s="22">
-        <f>COUNTIF(All_unique!B:B,B12)</f>
+      <c r="E12" s="22">
+        <f>COUNTIF(All_unique!B:B,C12)</f>
         <v>28</v>
       </c>
-      <c r="D12" s="22">
-        <f>COUNTIF(All!B:B,B12)</f>
+      <c r="F12" s="22">
+        <f>COUNTIF(All!B:B,C12)</f>
         <v>33</v>
       </c>
-      <c r="E12" s="22">
+      <c r="G12" s="22">
         <f>Details_old!F230</f>
         <v>20</v>
       </c>
-      <c r="F12" s="22">
+      <c r="H12" s="22">
         <f>Details_old!G230</f>
         <v>0</v>
       </c>
-      <c r="G12" s="22">
+      <c r="I12" s="22">
         <f>Details_old!H230</f>
         <v>20</v>
       </c>
-      <c r="H12" s="24">
+      <c r="J12" s="24">
         <f t="shared" si="0"/>
         <v>3.3333333333333335</v>
       </c>
-      <c r="J12" s="26" t="s">
+      <c r="K12" s="26" t="s">
         <v>354</v>
       </c>
-      <c r="K12" s="27">
+      <c r="L12" s="27">
         <v>0.91666666666666663</v>
       </c>
-      <c r="L12" s="27">
+      <c r="M12" s="27">
         <v>0.95833333333333337</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="15">
-      <c r="A13" s="22" t="s">
+    <row r="13" spans="1:13" ht="15">
+      <c r="A13" s="28">
+        <v>12</v>
+      </c>
+      <c r="B13" s="22" t="s">
         <v>369</v>
       </c>
-      <c r="B13" s="23" t="s">
+      <c r="C13" s="23" t="s">
         <v>291</v>
       </c>
-      <c r="C13" s="22">
-        <f>COUNTIF(All_unique!B:B,B13)</f>
+      <c r="E13" s="22">
+        <f>COUNTIF(All_unique!B:B,C13)</f>
         <v>2</v>
       </c>
-      <c r="D13" s="22">
-        <f>COUNTIF(All!B:B,B13)</f>
+      <c r="F13" s="22">
+        <f>COUNTIF(All!B:B,C13)</f>
         <v>26</v>
       </c>
-      <c r="E13" s="22">
+      <c r="G13" s="22">
         <f>Details_old!F336</f>
         <v>21</v>
       </c>
-      <c r="F13" s="22">
+      <c r="H13" s="22">
         <f>Details_old!G336</f>
         <v>0</v>
       </c>
-      <c r="G13" s="22">
+      <c r="I13" s="22">
         <f>Details_old!H336</f>
         <v>21</v>
       </c>
-      <c r="H13" s="24">
+      <c r="J13" s="24">
         <f t="shared" si="0"/>
         <v>3.5</v>
       </c>
-      <c r="J13" s="26" t="s">
+      <c r="K13" s="26" t="s">
         <v>354</v>
       </c>
-      <c r="K13" s="27">
+      <c r="L13" s="27">
         <v>0.70833333333333337</v>
       </c>
-      <c r="L13" s="27">
+      <c r="M13" s="27">
         <v>0.75</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="15">
-      <c r="A14" s="22" t="s">
+    <row r="14" spans="1:13" ht="15">
+      <c r="A14" s="28">
+        <v>13</v>
+      </c>
+      <c r="B14" s="22" t="s">
         <v>368</v>
       </c>
-      <c r="B14" s="23" t="s">
+      <c r="C14" s="23" t="s">
         <v>516</v>
       </c>
-      <c r="C14" s="22">
-        <f>COUNTIF(All_unique!B:B,B14)</f>
+      <c r="E14" s="22">
+        <f>COUNTIF(All_unique!B:B,C14)</f>
         <v>33</v>
       </c>
-      <c r="D14" s="22">
-        <f>COUNTIF(All!B:B,B14)</f>
+      <c r="F14" s="22">
+        <f>COUNTIF(All!B:B,C14)</f>
         <v>34</v>
       </c>
-      <c r="E14" s="22">
+      <c r="G14" s="22">
         <f>Details_old!F305</f>
         <v>30</v>
       </c>
-      <c r="F14" s="22">
+      <c r="H14" s="22">
         <f>Details_old!G305</f>
         <v>0</v>
       </c>
-      <c r="G14" s="22">
+      <c r="I14" s="22">
         <f>Details_old!H305</f>
         <v>30</v>
       </c>
-      <c r="H14" s="24">
+      <c r="J14" s="24">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="J14" s="26" t="s">
+      <c r="K14" s="26" t="s">
         <v>354</v>
       </c>
-      <c r="K14" s="27">
+      <c r="L14" s="27">
         <v>0.75</v>
       </c>
-      <c r="L14" s="27">
+      <c r="M14" s="27">
         <v>0.79166666666666663</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="15">
-      <c r="A15" s="22" t="s">
+    <row r="15" spans="1:13" ht="15">
+      <c r="A15" s="28">
+        <v>14</v>
+      </c>
+      <c r="B15" s="22" t="s">
         <v>359</v>
       </c>
-      <c r="B15" s="23" t="s">
+      <c r="C15" s="23" t="s">
         <v>292</v>
       </c>
-      <c r="C15" s="22">
-        <f>COUNTIF(All_unique!B:B,B15)</f>
+      <c r="E15" s="22">
+        <f>COUNTIF(All_unique!B:B,C15)</f>
         <v>6</v>
       </c>
-      <c r="D15" s="22">
-        <f>COUNTIF(All!B:B,B15)</f>
+      <c r="F15" s="22">
+        <f>COUNTIF(All!B:B,C15)</f>
         <v>44</v>
       </c>
-      <c r="E15" s="22">
+      <c r="G15" s="22">
         <f>Details_old!F90</f>
         <v>34</v>
       </c>
-      <c r="F15" s="22">
+      <c r="H15" s="22">
         <f>Details_old!G90</f>
         <v>0</v>
       </c>
-      <c r="G15" s="22">
+      <c r="I15" s="22">
         <f>Details_old!H90</f>
         <v>34</v>
       </c>
-      <c r="H15" s="24">
+      <c r="J15" s="24">
         <f t="shared" si="0"/>
         <v>5.666666666666667</v>
       </c>
-      <c r="J15" s="26" t="s">
+      <c r="K15" s="26" t="s">
         <v>354</v>
       </c>
-      <c r="K15" s="27">
+      <c r="L15" s="27">
         <v>0.79166666666666663</v>
       </c>
-      <c r="L15" s="27">
+      <c r="M15" s="27">
         <v>0.83333333333333337</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="15">
-      <c r="A16" s="22" t="s">
+    <row r="16" spans="1:13" ht="15">
+      <c r="A16" s="28">
+        <v>15</v>
+      </c>
+      <c r="B16" s="22" t="s">
         <v>370</v>
       </c>
-      <c r="B16" s="23" t="s">
+      <c r="C16" s="23" t="s">
         <v>303</v>
       </c>
-      <c r="C16" s="22">
-        <f>COUNTIF(All_unique!B:B,B16)</f>
+      <c r="E16" s="22">
+        <f>COUNTIF(All_unique!B:B,C16)</f>
         <v>43</v>
       </c>
-      <c r="D16" s="22">
-        <f>COUNTIF(All!B:B,B16)</f>
+      <c r="F16" s="22">
+        <f>COUNTIF(All!B:B,C16)</f>
         <v>72</v>
       </c>
-      <c r="E16" s="22">
+      <c r="G16" s="22">
         <f>Details_old!F358</f>
         <v>51</v>
       </c>
-      <c r="F16" s="22">
+      <c r="H16" s="22">
         <f>Details_old!G358</f>
         <v>2</v>
       </c>
-      <c r="G16" s="22">
+      <c r="I16" s="22">
         <f>Details_old!H358</f>
         <v>49</v>
       </c>
-      <c r="H16" s="24">
+      <c r="J16" s="24">
         <f t="shared" si="0"/>
         <v>8.5</v>
       </c>
-      <c r="J16" s="26" t="s">
+      <c r="K16" s="26" t="s">
         <v>354</v>
       </c>
-      <c r="K16" s="27">
+      <c r="L16" s="27">
         <v>0.83333333333333337</v>
       </c>
-      <c r="L16" s="27">
+      <c r="M16" s="27">
         <v>0.875</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="15">
-      <c r="A17" s="22" t="s">
+    <row r="17" spans="1:13" ht="15">
+      <c r="A17" s="28">
+        <v>16</v>
+      </c>
+      <c r="B17" s="22" t="s">
         <v>364</v>
       </c>
-      <c r="B17" s="23" t="s">
+      <c r="C17" s="23" t="s">
         <v>272</v>
       </c>
-      <c r="C17" s="22">
-        <f>COUNTIF(All_unique!B:B,B17)</f>
+      <c r="E17" s="22">
+        <f>COUNTIF(All_unique!B:B,C17)</f>
         <v>21</v>
       </c>
-      <c r="D17" s="22">
-        <f>COUNTIF(All!B:B,B17)</f>
+      <c r="F17" s="22">
+        <f>COUNTIF(All!B:B,C17)</f>
         <v>37</v>
       </c>
-      <c r="E17" s="22">
+      <c r="G17" s="22">
         <f>Details_old!F196</f>
         <v>33</v>
       </c>
-      <c r="F17" s="22">
+      <c r="H17" s="22">
         <f>Details_old!G196</f>
         <v>0</v>
       </c>
-      <c r="G17" s="22">
+      <c r="I17" s="22">
         <f>Details_old!H196</f>
         <v>33</v>
       </c>
-      <c r="H17" s="24">
-        <f>E17*10/60</f>
+      <c r="J17" s="24">
+        <f t="shared" si="0"/>
         <v>5.5</v>
       </c>
-      <c r="J17" s="26" t="s">
+      <c r="K17" s="26" t="s">
         <v>354</v>
       </c>
-      <c r="K17" s="27">
+      <c r="L17" s="27">
         <v>0.875</v>
       </c>
-      <c r="L17" s="27">
+      <c r="M17" s="27">
         <v>0.91666666666666663</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="15">
-      <c r="A18" s="22" t="s">
+    <row r="18" spans="1:13" ht="15">
+      <c r="A18" s="28">
+        <v>17</v>
+      </c>
+      <c r="B18" s="22" t="s">
         <v>361</v>
       </c>
-      <c r="B18" s="29" t="s">
+      <c r="C18" s="29" t="s">
         <v>213</v>
       </c>
-      <c r="C18" s="22">
-        <f>COUNTIF(All_unique!B:B,B18)</f>
+      <c r="E18" s="22">
+        <f>COUNTIF(All_unique!B:B,C18)</f>
         <v>31</v>
       </c>
-      <c r="D18" s="22">
-        <f>COUNTIF(All!B:B,B18)</f>
+      <c r="F18" s="22">
+        <f>COUNTIF(All!B:B,C18)</f>
         <v>35</v>
       </c>
-      <c r="E18" s="22">
+      <c r="G18" s="22">
         <f>Details_old!F142</f>
         <v>29</v>
       </c>
-      <c r="F18" s="22">
+      <c r="H18" s="22">
         <f>Details_old!G142</f>
         <v>0</v>
       </c>
-      <c r="G18" s="22">
+      <c r="I18" s="22">
         <f>Details_old!H142</f>
         <v>29</v>
       </c>
-      <c r="H18" s="24">
-        <f>E18*10/60</f>
+      <c r="J18" s="24">
+        <f t="shared" si="0"/>
         <v>4.833333333333333</v>
       </c>
-      <c r="J18" s="26" t="s">
+      <c r="K18" s="26" t="s">
         <v>354</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="15">
-      <c r="A19" s="22" t="s">
+    <row r="19" spans="1:13" ht="15">
+      <c r="A19" s="28">
+        <v>18</v>
+      </c>
+      <c r="B19" s="22" t="s">
         <v>372</v>
       </c>
-      <c r="B19" s="23" t="s">
-        <v>0</v>
-      </c>
-      <c r="C19" s="22">
-        <f>COUNTIF(All_unique!B:B,B19)</f>
+      <c r="C19" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="E19" s="22">
+        <f>COUNTIF(All_unique!B:B,C19)</f>
         <v>125</v>
       </c>
-      <c r="D19" s="22">
-        <f>COUNTIF(All!B:B,B19)</f>
+      <c r="F19" s="22">
+        <f>COUNTIF(All!B:B,C19)</f>
         <v>125</v>
       </c>
-      <c r="E19" s="22">
+      <c r="G19" s="22">
         <f>Details_old!F424</f>
         <v>92</v>
       </c>
-      <c r="F19" s="22">
+      <c r="H19" s="22">
         <f>Details_old!G424</f>
         <v>0</v>
       </c>
-      <c r="G19" s="22">
+      <c r="I19" s="22">
         <f>Details_old!H424</f>
         <v>92</v>
       </c>
-      <c r="H19" s="24">
+      <c r="J19" s="24">
         <f t="shared" si="0"/>
         <v>15.333333333333334</v>
       </c>
-      <c r="J19" s="26" t="s">
+      <c r="K19" s="26" t="s">
         <v>522</v>
       </c>
     </row>
-    <row r="21" spans="1:12" s="15" customFormat="1" ht="15">
-      <c r="B21" s="16" t="s">
+    <row r="21" spans="1:13" s="15" customFormat="1" ht="15">
+      <c r="C21" s="16" t="s">
         <v>374</v>
       </c>
-      <c r="C21" s="16">
-        <f>SUM(C2:C20)</f>
+      <c r="D21" s="18"/>
+      <c r="E21" s="16">
+        <f t="shared" ref="E21:J21" si="1">SUM(E2:E20)</f>
         <v>438</v>
       </c>
-      <c r="D21" s="16">
-        <f t="shared" ref="D21:H21" si="1">SUM(D2:D20)</f>
+      <c r="F21" s="16">
+        <f t="shared" si="1"/>
         <v>644</v>
       </c>
-      <c r="E21" s="16">
+      <c r="G21" s="16">
         <f t="shared" si="1"/>
         <v>497</v>
       </c>
-      <c r="F21" s="16">
+      <c r="H21" s="16">
         <f t="shared" si="1"/>
         <v>57</v>
       </c>
-      <c r="G21" s="16">
+      <c r="I21" s="16">
         <f t="shared" si="1"/>
         <v>440</v>
       </c>
-      <c r="H21" s="17">
+      <c r="J21" s="17">
         <f t="shared" si="1"/>
         <v>82.833333333333329</v>
       </c>
-      <c r="I21" s="18"/>
-      <c r="J21" s="19"/>
+      <c r="K21" s="19"/>
     </row>
   </sheetData>
-  <sortState ref="A2:G19">
-    <sortCondition ref="E3:E19"/>
+  <sortState ref="A2:N21">
+    <sortCondition ref="G3:G19"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -30506,7 +30580,7 @@
   </sheetPr>
   <dimension ref="A1:L518"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>

</xml_diff>